<commit_message>
added additional example stimuli and updated spreadsheet accordingly
</commit_message>
<xml_diff>
--- a/Stimuli_key.xlsx
+++ b/Stimuli_key.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haleyfrey/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haleyfrey/Desktop/Supplementary Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1C13FC-0CE3-864A-8C1E-174EAA1F4832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57227C54-EF14-9848-B639-6C71E6352FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="500" windowWidth="28220" windowHeight="16340" xr2:uid="{A16CD5F5-3D4C-5C45-B09E-6BB6C40236B7}"/>
+    <workbookView xWindow="180" yWindow="500" windowWidth="17540" windowHeight="16340" xr2:uid="{A16CD5F5-3D4C-5C45-B09E-6BB6C40236B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="YellowOrange" sheetId="1" r:id="rId1"/>
+    <sheet name="BluePurple" sheetId="2" r:id="rId2"/>
+    <sheet name="PurpleOrange" sheetId="3" r:id="rId3"/>
+    <sheet name="PurpleOrange-NonStandard" sheetId="5" r:id="rId4"/>
+    <sheet name="BlueYellow" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="92">
   <si>
     <t>Img02_BluePurple</t>
   </si>
@@ -231,6 +235,87 @@
   </si>
   <si>
     <t>window appears</t>
+  </si>
+  <si>
+    <t>Img02_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Img03_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Img04_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Img05_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Img06_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Img07_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Img10_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Img09_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Img08_PurpleOrange</t>
+  </si>
+  <si>
+    <t>Birds diappear, middle girl's head changes right to left, fish disappears</t>
+  </si>
+  <si>
+    <t>girl disappears, middle mountain gains texture</t>
+  </si>
+  <si>
+    <t>tattoo appears, skirt lengthens</t>
+  </si>
+  <si>
+    <t>plant disappears on left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rocket changes right to left, bag changes green to pink, radio disappears </t>
+  </si>
+  <si>
+    <t>clock appears, frown to smile, lamp appears</t>
+  </si>
+  <si>
+    <t>girl disappears, middle mountain loses texture</t>
+  </si>
+  <si>
+    <t>clock flips upside down, pencil disappears</t>
+  </si>
+  <si>
+    <t>stars disappear from top, red ball gets larger</t>
+  </si>
+  <si>
+    <t>Img02_BlueYellow</t>
+  </si>
+  <si>
+    <t>Img03_BlueYellow</t>
+  </si>
+  <si>
+    <t>Img04_BlueYellow</t>
+  </si>
+  <si>
+    <t>Img05_BlueYellow</t>
+  </si>
+  <si>
+    <t>Img07_BlueYellow</t>
+  </si>
+  <si>
+    <t>Img06_BlueYellow</t>
+  </si>
+  <si>
+    <t>Img08_BlueYellow</t>
+  </si>
+  <si>
+    <t>Img09_BlueYellow</t>
+  </si>
+  <si>
+    <t>Img10_BlueYellow</t>
   </si>
 </sst>
 </file>
@@ -593,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10D9865-8E56-BF45-837A-F56E6DDC72F8}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,13 +716,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -651,341 +736,1053 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>61</v>
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>61</v>
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
-        <v>34</v>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
+      <c r="A7" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC021365-D39F-C04C-B908-953E167CB6EA}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A2:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>39</v>
       </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07529EF7-F583-2E4D-ADF0-F73A6202557E}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2220E9-63C5-AF4B-9856-E8EBC1DABCE2}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0E69AD-50F1-0043-8A36-10BCECE6E4B3}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>34</v>
       </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>53</v>
+      <c r="A10" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>51</v>
+      <c r="E10" t="s">
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>